<commit_message>
finalize job after code review
</commit_message>
<xml_diff>
--- a/docs/Planification.xlsx
+++ b/docs/Planification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chapuisbertil/Projects/github.com/isplab-unil/commoncrawl-sri/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3C1748-01AF-8740-8904-454BA70DE896}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451401E2-6660-6B47-985D-633EFCA428FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{96E31602-DBE7-3B40-B9BA-3B1BDC983095}"/>
   </bookViews>
@@ -23,12 +23,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>warc</t>
   </si>
@@ -501,26 +507,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B741595-8E0B-6E42-81B0-4DDCC8A2903A}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="10.83203125" style="2"/>
-    <col min="8" max="8" width="3.33203125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="2" max="8" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="3.33203125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -528,7 +534,7 @@
         <v>65500</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -539,7 +545,7 @@
         <v>0.192</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -550,10 +556,10 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -575,8 +581,11 @@
       <c r="G8" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="3">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -598,8 +607,11 @@
       <c r="G9" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="3">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -621,8 +633,11 @@
       <c r="G10" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -644,8 +659,11 @@
       <c r="G11" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -667,8 +685,11 @@
       <c r="G12" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -696,8 +717,12 @@
         <f>SUM(G10:G12)</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" s="4">
+        <f>SUM(H10:H12)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -725,8 +750,12 @@
         <f>1/60*35</f>
         <v>0.58333333333333337</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" s="5">
+        <f>1/60*35</f>
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -747,15 +776,19 @@
         <v>0.37440000000000007</v>
       </c>
       <c r="F15" s="8">
-        <f>F14*SUM(F10:F11)*$C5+F12*G6</f>
+        <f>F14*SUM(F10:F11)*$C5+F12*H6</f>
         <v>0.34559999999999996</v>
       </c>
       <c r="G15" s="8">
         <f>G14*SUM(G10:G11)*$C5+G12*H6</f>
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" s="8">
+        <f>H14*SUM(H10:H11)*$C5+H12*I6</f>
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -777,8 +810,11 @@
       <c r="G16" s="5">
         <v>431</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H16" s="5">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
@@ -806,16 +842,20 @@
         <f>G14/G8*warc_files/24</f>
         <v>15.920138888888891</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="H17" s="8">
+        <f>H14/H8*warc_files/24</f>
+        <v>2.8428819444444446</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="4">
-        <f t="shared" ref="B18:G18" si="1">B15/B8*warc_files</f>
+        <f t="shared" ref="B18:H18" si="1">B15/B8*warc_files</f>
         <v>1970.2400000000002</v>
       </c>
       <c r="C18" s="8">
@@ -835,14 +875,18 @@
         <v>452.73599999999993</v>
       </c>
       <c r="G18" s="8">
+        <f t="shared" ref="G18" si="2">G15/G8*warc_files</f>
+        <v>366.80000000000007</v>
+      </c>
+      <c r="H18" s="8">
         <f t="shared" si="1"/>
-        <v>366.80000000000007</v>
-      </c>
-      <c r="I18" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
@@ -865,46 +909,54 @@
         <f>G16/G8*warc_files</f>
         <v>282305</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="H19" s="8">
+        <f>H16/H8*warc_files</f>
+        <v>50411.607142857145</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="91" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="91" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="6" t="str">
-        <f>_xlfn.CONCAT("./submit-remote.py full.py ", B8, "_warc.txt ", B9, " ", B10, " ", B11, " ", B12)</f>
+        <f t="shared" ref="B21:H21" si="3">_xlfn.CONCAT("./submit-remote.py full.py ", B8, "_warc.txt ", B9, " ", B10, " ", B11, " ", B12)</f>
         <v>./submit-remote.py full.py 10_warc.txt 10 1 1 0</v>
       </c>
       <c r="C21" s="6" t="str">
-        <f>_xlfn.CONCAT("./submit-remote.py full.py ", C8, "_warc.txt ", C9, " ", C10, " ", C11, " ", C12)</f>
+        <f t="shared" si="3"/>
         <v>./submit-remote.py full.py 20_warc.txt 20 1 1 2</v>
       </c>
       <c r="D21" s="6" t="str">
-        <f>_xlfn.CONCAT("./submit-remote.py full.py ", D8, "_warc.txt ", D9, " ", D10, " ", D11, " ", D12)</f>
+        <f t="shared" si="3"/>
         <v>./submit-remote.py full.py 30_warc.txt 30 1 2 3</v>
       </c>
       <c r="E21" s="6" t="str">
-        <f>_xlfn.CONCAT("./submit-remote.py full.py ", E8, "_warc.txt ", E9, " ", E10, " ", E11, " ", E12)</f>
+        <f t="shared" si="3"/>
         <v>./submit-remote.py full.py 40_warc.txt 40 1 2 5</v>
       </c>
       <c r="F21" s="6" t="str">
-        <f>_xlfn.CONCAT("./submit-remote.py full.py ", F8, "_warc.txt ", F9, " ", F10, " ", F11, " ", F12)</f>
+        <f t="shared" si="3"/>
         <v>./submit-remote.py full.py 50_warc.txt 50 1 2 7</v>
       </c>
       <c r="G21" s="6" t="str">
-        <f>_xlfn.CONCAT("./submit-remote.py full.py ", G8, "_warc.txt ", G9, " ", G10, " ", G11, " ", G12)</f>
+        <f t="shared" ref="G21" si="4">_xlfn.CONCAT("./submit-remote.py full.py ", G8, "_warc.txt ", G9, " ", G10, " ", G11, " ", G12)</f>
         <v>./submit-remote.py full.py 100_warc.txt 100 1 4 15</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="H21" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>./submit-remote.py full.py 560_warc.txt 560 1 9 30</v>
+      </c>
+      <c r="J21" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
     </row>
-    <row r="23" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>10</v>
       </c>
@@ -926,8 +978,11 @@
       <c r="G23" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H23" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
     </row>
   </sheetData>

</xml_diff>